<commit_message>
adding most recent instrument deployment info
</commit_message>
<xml_diff>
--- a/environmental_data/instrument_deployment_info.xlsx
+++ b/environmental_data/instrument_deployment_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://miamiedu-my.sharepoint.com/personal/and128_miami_edu/Documents/GitHub/Ch3_reciprocaltransplant/environmental_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allyson.demerlis/Documents/GitHub/Ch3_reciprocaltransplant/environmental_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{E5486F79-C23E-F144-975E-D0F30905F1F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{970F8BA7-0096-074B-80A8-25C90300B560}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729FFF6C-E480-944A-89F2-755E7510EB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31000" yWindow="500" windowWidth="30100" windowHeight="20220" xr2:uid="{1EDCCD75-4C6C-A347-8B2B-E208347A7CDC}"/>
+    <workbookView xWindow="8960" yWindow="1860" windowWidth="38020" windowHeight="21140" xr2:uid="{1EDCCD75-4C6C-A347-8B2B-E208347A7CDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="23">
   <si>
     <t>Type</t>
   </si>
@@ -150,13 +149,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,13 +469,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF98029E-D6B1-014F-8802-83DBA4C402EF}">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="9" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -545,6 +548,12 @@
       <c r="H2" s="1">
         <v>24</v>
       </c>
+      <c r="I2" s="4">
+        <v>45250</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -571,6 +580,12 @@
       <c r="H3" s="1">
         <v>5</v>
       </c>
+      <c r="I3" s="4">
+        <v>45250</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -597,6 +612,12 @@
       <c r="H4" s="1">
         <v>5</v>
       </c>
+      <c r="I4" s="4">
+        <v>45250</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -623,6 +644,12 @@
       <c r="H5" s="1">
         <v>24</v>
       </c>
+      <c r="I5" s="4">
+        <v>45250</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -1028,7 +1055,7 @@
       <c r="H19" s="1">
         <v>20</v>
       </c>
-      <c r="I19" s="5">
+      <c r="I19" s="4">
         <v>45118</v>
       </c>
       <c r="J19" s="1" t="s">
@@ -1057,7 +1084,7 @@
       <c r="H20" s="1">
         <v>5</v>
       </c>
-      <c r="I20" s="5">
+      <c r="I20" s="4">
         <v>45118</v>
       </c>
       <c r="J20" s="1" t="s">
@@ -1077,19 +1104,19 @@
       <c r="E21" s="4">
         <v>45020</v>
       </c>
-      <c r="I21" s="5">
+      <c r="I21" s="4">
         <v>45118</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="1">
         <v>6635</v>
       </c>
-      <c r="L21" t="s">
-        <v>14</v>
-      </c>
-      <c r="M21" s="5">
+      <c r="L21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M21" s="4">
         <v>45121</v>
       </c>
     </row>
@@ -1106,19 +1133,19 @@
       <c r="E22" s="4">
         <v>45020</v>
       </c>
-      <c r="I22" s="5">
+      <c r="I22" s="4">
         <v>45118</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="1">
         <v>7398</v>
       </c>
-      <c r="L22" t="s">
-        <v>15</v>
-      </c>
-      <c r="M22" s="5">
+      <c r="L22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M22" s="4">
         <v>45121</v>
       </c>
     </row>
@@ -1135,19 +1162,19 @@
       <c r="E23" s="4">
         <v>45020</v>
       </c>
-      <c r="I23" s="5">
+      <c r="I23" s="4">
         <v>45118</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="1">
         <v>4298</v>
       </c>
-      <c r="L23" t="s">
-        <v>14</v>
-      </c>
-      <c r="M23" s="5">
+      <c r="L23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M23" s="4">
         <v>45121</v>
       </c>
     </row>
@@ -1164,19 +1191,19 @@
       <c r="E24" s="4">
         <v>45020</v>
       </c>
-      <c r="I24" s="5">
+      <c r="I24" s="4">
         <v>45118</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="1">
         <v>4297</v>
       </c>
-      <c r="L24" t="s">
-        <v>15</v>
-      </c>
-      <c r="M24" s="5">
+      <c r="L24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M24" s="4">
         <v>45121</v>
       </c>
     </row>
@@ -1190,8 +1217,14 @@
       <c r="D25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="4">
         <v>45121</v>
+      </c>
+      <c r="I25" s="4">
+        <v>45250</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -1202,10 +1235,96 @@
         <v>4299</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="5">
+        <v>15</v>
+      </c>
+      <c r="E26" s="4">
         <v>45121</v>
+      </c>
+      <c r="I26" s="4">
+        <v>45250</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="1">
+        <v>6635</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="4">
+        <v>45121</v>
+      </c>
+      <c r="I27" s="4">
+        <v>45250</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="1">
+        <v>7398</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="4">
+        <v>45121</v>
+      </c>
+      <c r="I28" s="4">
+        <v>45250</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="1">
+        <v>4298</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="4">
+        <v>45121</v>
+      </c>
+      <c r="I29" s="4">
+        <v>45250</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="1">
+        <v>4297</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="4">
+        <v>45121</v>
+      </c>
+      <c r="I30" s="4">
+        <v>45250</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>